<commit_message>
rename column's datatype, name + add more func
rename column's datatype, name + add more func
</commit_message>
<xml_diff>
--- a/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
+++ b/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>플래너</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -194,10 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bigint</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>varchar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -263,6 +259,14 @@
   </si>
   <si>
     <t>endDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nowDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -848,7 +852,7 @@
   <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.3"/>
@@ -961,7 +965,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -972,7 +976,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1016,10 +1020,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -1033,10 +1037,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -1141,7 +1145,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
@@ -1152,98 +1156,98 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2">
         <v>100</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" s="2"/>
     </row>

</xml_diff>

<commit_message>
move all things to sb_sbsj KJS_Planner branch
move all things to sb_sbsj KJS_Planner branch
</commit_message>
<xml_diff>
--- a/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
+++ b/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>플래너</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,10 +226,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이디</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,6 +263,22 @@
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>planId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>planSpId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA를 잊어라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mybatis 사용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -851,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.3"/>
@@ -965,7 +977,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -976,7 +988,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1020,7 +1032,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>41</v>
@@ -1037,7 +1049,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
@@ -1091,6 +1103,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H16" s="4"/>
@@ -1145,7 +1165,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
@@ -1156,14 +1176,14 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
@@ -1181,7 +1201,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>42</v>
@@ -1200,10 +1220,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
@@ -1211,13 +1231,13 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>42</v>
@@ -1236,7 +1256,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
nowDate -> spotDate & whatDay 미사용
nowDate -> spotDate & whatDay 미사용
</commit_message>
<xml_diff>
--- a/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
+++ b/table/상부상조팀프로젝트데이터설계_강준서(플래너).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>플래너</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,10 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bigint</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -162,10 +158,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>작성자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>memo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -258,10 +250,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nowDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -279,6 +267,22 @@
   </si>
   <si>
     <t>Mybatis 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자 ID 값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spotDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 사용 x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -286,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +327,14 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -489,7 +501,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,6 +558,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,7 +879,7 @@
   <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.3"/>
@@ -940,7 +955,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="9" t="s">
@@ -977,10 +992,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -988,16 +1003,16 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
         <v>100</v>
@@ -1007,35 +1022,33 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2">
-        <v>20</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -1043,16 +1056,16 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -1060,35 +1073,35 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <v>100</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -1096,7 +1109,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="4"/>
@@ -1106,10 +1119,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1125,14 +1138,14 @@
         <v>16</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="14"/>
@@ -1165,10 +1178,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
@@ -1176,98 +1189,100 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2">
         <v>100</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G25" s="2"/>
     </row>

</xml_diff>